<commit_message>
Minor cleanup of code
</commit_message>
<xml_diff>
--- a/BOM_Processor/20240322-Electrical component library.xlsx
+++ b/BOM_Processor/20240322-Electrical component library.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Components" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Components!$B$6:$M$134</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Components!$B$6:$M$143</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="551">
   <si>
     <t xml:space="preserve">Document:</t>
   </si>
@@ -337,6 +337,9 @@
     <t xml:space="preserve">1k</t>
   </si>
   <si>
+    <t xml:space="preserve">25%</t>
+  </si>
+  <si>
     <t xml:space="preserve">350mA</t>
   </si>
   <si>
@@ -1574,6 +1577,105 @@
   </si>
   <si>
     <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Texas-Instruments/LM321LVIDCKR?qs=qSfuJ%252Bfl%2Fd6RcyTOjkRx5Q%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS636_SL50_SMTR_LFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C&amp;K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/CK/PTS636-SL50-SMTR-LFS?qs=vLWxofP3U2zRoRV76Po6zQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP7113ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.9V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Kingbright/WP7113ID?qs=hyavMCx%252BcmDJhCThgY7pfQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLM18KG101TN1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Murata-Electronics/BLM18KG101TN1D?qs=MY6wChARw2zdno9LTSL6Ng%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAY16-681J4LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4x1603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Bourns/CAY16-681J4LF?qs=fd0Ij%252BN8svzpg8SscutFRQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PESD5Z5.0F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Nexperia/PESD5Z5.0F?qs=HNBw3F7vE2wb3Eh3cMl6Jg%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP7113ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.95V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Kingbright/WP7113ND?qs=CJFmpBjNieP5MCFQ3vDfmg%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP7113GD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Kingbright/WP7113GD?qs=pz0eHrWKk7njL1kTYKysuw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTINY9-TS8R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10Mhz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1kB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.mouser.com/ProductDetail/Microchip-Technology/ATTINY9-TS8R?qs=%2Fqzd9s%252BcLd6Ex7DNcGSsRA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -2169,12 +2271,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:M134"/>
+  <dimension ref="B2:M142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="6" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E138" activeCellId="0" sqref="E138"/>
+      <selection pane="bottomLeft" activeCell="C149" activeCellId="0" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2640,17 +2742,17 @@
       <c r="F20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="2" t="n">
-        <v>0.25</v>
+      <c r="G20" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L20" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,19 +2760,19 @@
         <v>79</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>76</v>
@@ -2679,56 +2781,56 @@
         <v>0.567</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L22" s="4" t="n">
         <v>0.837</v>
       </c>
       <c r="M22" s="21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L23" s="4" t="n">
         <v>0.307</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,13 +2838,13 @@
         <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>69</v>
@@ -2751,7 +2853,7 @@
         <v>0.353</v>
       </c>
       <c r="M24" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,7 +2861,7 @@
         <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>56</v>
@@ -2768,13 +2870,13 @@
         <v>57</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L25" s="4" t="n">
         <v>0.428</v>
       </c>
       <c r="M25" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2782,10 +2884,10 @@
         <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>20</v>
@@ -2803,7 +2905,7 @@
         <v>0.093</v>
       </c>
       <c r="M26" s="21" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,28 +2913,28 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L27" s="4" t="n">
         <v>0.233</v>
       </c>
       <c r="M27" s="21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,28 +2942,28 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L28" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2971,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>102</v>
@@ -2878,19 +2980,19 @@
         <v>95</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L29" s="4" t="n">
         <v>0.335</v>
       </c>
       <c r="M29" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2898,28 +3000,28 @@
         <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L30" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M30" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,7 +3029,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>102</v>
@@ -2936,19 +3038,19 @@
         <v>20</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L31" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M31" s="21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,10 +3058,10 @@
         <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>20</v>
@@ -2980,7 +3082,7 @@
         <v>0.093</v>
       </c>
       <c r="M32" s="21" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,10 +3090,10 @@
         <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>20</v>
@@ -3012,7 +3114,7 @@
         <v>0.093</v>
       </c>
       <c r="M33" s="21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,16 +3122,16 @@
         <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>97</v>
@@ -3044,7 +3146,7 @@
         <v>0.093</v>
       </c>
       <c r="M34" s="21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,16 +3154,16 @@
         <v>17</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>97</v>
@@ -3076,7 +3178,7 @@
         <v>0.093</v>
       </c>
       <c r="M35" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3084,16 +3186,16 @@
         <v>17</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>97</v>
@@ -3108,7 +3210,7 @@
         <v>0.093</v>
       </c>
       <c r="M36" s="21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3116,16 +3218,16 @@
         <v>17</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>97</v>
@@ -3140,7 +3242,7 @@
         <v>0.093</v>
       </c>
       <c r="M37" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,16 +3250,16 @@
         <v>17</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>97</v>
@@ -3166,13 +3268,13 @@
         <v>23</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L38" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M38" s="21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3180,10 +3282,10 @@
         <v>17</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>20</v>
@@ -3204,7 +3306,7 @@
         <v>0.093</v>
       </c>
       <c r="M39" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3212,10 +3314,10 @@
         <v>17</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>20</v>
@@ -3236,7 +3338,7 @@
         <v>0.112</v>
       </c>
       <c r="M40" s="21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,7 +3346,7 @@
         <v>17</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>94</v>
@@ -3253,7 +3355,7 @@
         <v>20</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>97</v>
@@ -3262,13 +3364,13 @@
         <v>23</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L41" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M41" s="21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,16 +3378,16 @@
         <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>30</v>
@@ -3297,7 +3399,7 @@
         <v>0.093</v>
       </c>
       <c r="M42" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,7 +3407,7 @@
         <v>60</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>62</v>
@@ -3314,10 +3416,10 @@
         <v>63</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>66</v>
@@ -3326,7 +3428,7 @@
         <v>0.177</v>
       </c>
       <c r="M43" s="21" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3334,7 +3436,7 @@
         <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>62</v>
@@ -3343,10 +3445,10 @@
         <v>63</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>66</v>
@@ -3355,7 +3457,7 @@
         <v>0.177</v>
       </c>
       <c r="M44" s="21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,7 +3465,7 @@
         <v>26</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>28</v>
@@ -3372,7 +3474,7 @@
         <v>20</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>22</v>
@@ -3384,7 +3486,7 @@
         <v>0.242</v>
       </c>
       <c r="M45" s="21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3392,10 +3494,10 @@
         <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>82</v>
@@ -3404,16 +3506,16 @@
         <v>88</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L46" s="4" t="n">
         <v>1.15</v>
       </c>
       <c r="M46" s="21" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,10 +3523,10 @@
         <v>100</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>95</v>
@@ -3432,17 +3534,17 @@
       <c r="F47" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="G47" s="2" t="n">
-        <v>0.25</v>
+      <c r="G47" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L47" s="4" t="n">
         <v>0.102</v>
       </c>
       <c r="M47" s="21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3450,13 +3552,13 @@
         <v>54</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>58</v>
@@ -3465,7 +3567,7 @@
         <v>0.353</v>
       </c>
       <c r="M48" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,10 +3575,10 @@
         <v>17</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>20</v>
@@ -3497,7 +3599,7 @@
         <v>0.093</v>
       </c>
       <c r="M49" s="21" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,10 +3607,10 @@
         <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>20</v>
@@ -3523,13 +3625,13 @@
         <v>23</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L50" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M50" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,51 +3639,51 @@
         <v>54</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="L51" s="4" t="n">
         <v>0.326</v>
       </c>
       <c r="M51" s="21" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L52" s="4" t="n">
         <v>0.186</v>
       </c>
       <c r="M52" s="21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,7 +3691,7 @@
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>102</v>
@@ -3604,13 +3706,13 @@
         <v>30</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L53" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3720,7 @@
         <v>17</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>19</v>
@@ -3627,7 +3729,7 @@
         <v>20</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>22</v>
@@ -3642,7 +3744,7 @@
         <v>0.093</v>
       </c>
       <c r="M54" s="21" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3650,28 +3752,28 @@
         <v>26</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L55" s="4" t="n">
         <v>0.27</v>
       </c>
       <c r="M55" s="21" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3679,10 +3781,10 @@
         <v>17</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>20</v>
@@ -3703,7 +3805,7 @@
         <v>0.093</v>
       </c>
       <c r="M56" s="21" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,10 +3813,10 @@
         <v>17</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>20</v>
@@ -3735,7 +3837,7 @@
         <v>0.093</v>
       </c>
       <c r="M57" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,80 +3845,80 @@
         <v>26</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L58" s="4" t="n">
         <v>0.093</v>
       </c>
       <c r="M58" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L59" s="4" t="n">
         <v>0.446</v>
       </c>
       <c r="M59" s="21" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="L60" s="4" t="n">
         <v>0.493</v>
       </c>
       <c r="M60" s="21" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,45 +3926,45 @@
         <v>54</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L61" s="4" t="n">
         <v>0.307</v>
       </c>
       <c r="M61" s="21" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L62" s="4" t="n">
         <v>0.446</v>
       </c>
       <c r="M62" s="21" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3870,51 +3972,51 @@
         <v>79</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L63" s="4" t="n">
         <v>0.577</v>
       </c>
       <c r="M63" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>58</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L64" s="4" t="n">
         <v>1.37</v>
       </c>
       <c r="M64" s="21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3922,13 +4024,13 @@
         <v>54</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>58</v>
@@ -3937,30 +4039,30 @@
         <v>0.353</v>
       </c>
       <c r="M65" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L66" s="4" t="n">
         <v>1.45</v>
       </c>
       <c r="M66" s="21" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3968,28 +4070,28 @@
         <v>60</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L67" s="4" t="n">
         <v>0.409</v>
       </c>
       <c r="M67" s="22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,7 +4099,7 @@
         <v>60</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>62</v>
@@ -4006,68 +4108,68 @@
         <v>63</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L68" s="4" t="n">
         <v>0.143</v>
       </c>
       <c r="M68" s="22" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L69" s="4" t="n">
         <v>0.095</v>
       </c>
       <c r="M69" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L70" s="4" t="n">
         <v>0.513</v>
       </c>
       <c r="M70" s="22" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4075,16 +4177,16 @@
         <v>17</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>97</v>
@@ -4099,7 +4201,7 @@
         <v>0.095</v>
       </c>
       <c r="M71" s="22" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4107,16 +4209,16 @@
         <v>17</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>97</v>
@@ -4131,111 +4233,111 @@
         <v>0.095</v>
       </c>
       <c r="M72" s="22" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>76</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L73" s="4" t="n">
         <v>0.371</v>
       </c>
       <c r="M73" s="22" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L74" s="4" t="n">
         <v>1.24</v>
       </c>
       <c r="M74" s="22" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L75" s="4" t="n">
         <v>0.304</v>
       </c>
       <c r="M75" s="22" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L76" s="4" t="n">
         <v>0.105</v>
       </c>
       <c r="M76" s="22" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4243,10 +4345,10 @@
         <v>79</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>82</v>
@@ -4255,7 +4357,7 @@
         <v>88</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>46</v>
@@ -4264,21 +4366,21 @@
         <v>0.494</v>
       </c>
       <c r="M77" s="22" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>58</v>
@@ -4287,13 +4389,13 @@
         <v>76</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L78" s="4" t="n">
         <v>0.209</v>
       </c>
       <c r="M78" s="22" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,74 +4403,74 @@
         <v>71</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>76</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L79" s="4" t="n">
         <v>1.68</v>
       </c>
       <c r="M79" s="22" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="L80" s="4" t="n">
         <v>6.54</v>
       </c>
       <c r="M80" s="22" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>23</v>
@@ -4377,7 +4479,7 @@
         <v>0.608</v>
       </c>
       <c r="M81" s="22" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4385,22 +4487,22 @@
         <v>54</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="L82" s="4" t="n">
         <v>0.38</v>
       </c>
       <c r="M82" s="22" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4408,28 +4510,28 @@
         <v>26</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L83" s="4" t="n">
         <v>0.095</v>
       </c>
       <c r="M83" s="22" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4437,28 +4539,28 @@
         <v>26</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L84" s="4" t="n">
         <v>0.19</v>
       </c>
       <c r="M84" s="22" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4466,28 +4568,28 @@
         <v>26</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L85" s="4" t="n">
         <v>0.181</v>
       </c>
       <c r="M85" s="22" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4495,19 +4597,19 @@
         <v>79</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>46</v>
@@ -4516,7 +4618,7 @@
         <v>0.266</v>
       </c>
       <c r="M86" s="22" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4524,13 +4626,13 @@
         <v>54</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>58</v>
@@ -4539,59 +4641,59 @@
         <v>0.114</v>
       </c>
       <c r="M87" s="22" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="L88" s="4" t="n">
         <v>0.608</v>
       </c>
       <c r="M88" s="22" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L89" s="4" t="n">
         <v>0.095</v>
       </c>
       <c r="M89" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,13 +4701,13 @@
         <v>54</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>58</v>
@@ -4614,7 +4716,7 @@
         <v>0.266</v>
       </c>
       <c r="M90" s="22" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4622,33 +4724,33 @@
         <v>79</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L91" s="4" t="n">
         <v>0.39</v>
       </c>
       <c r="M91" s="22" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>82</v>
@@ -4657,13 +4759,13 @@
         <v>91</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L92" s="4" t="n">
         <v>0.295</v>
       </c>
       <c r="M92" s="22" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4671,16 +4773,16 @@
         <v>17</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>97</v>
@@ -4695,33 +4797,33 @@
         <v>0.095</v>
       </c>
       <c r="M93" s="22" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L94" s="4" t="n">
         <v>0.257</v>
       </c>
       <c r="M94" s="22" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4729,19 +4831,19 @@
         <v>33</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>38</v>
@@ -4750,36 +4852,36 @@
         <v>8.41</v>
       </c>
       <c r="M95" s="22" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L96" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="M96" s="22" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4787,54 +4889,54 @@
         <v>26</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L97" s="4" t="n">
         <v>0.475</v>
       </c>
       <c r="M97" s="22" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L98" s="4" t="n">
         <v>0.599</v>
       </c>
       <c r="M98" s="22" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,54 +4944,54 @@
         <v>26</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L99" s="4" t="n">
         <v>0.722</v>
       </c>
       <c r="M99" s="22" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="L100" s="4" t="n">
         <v>0.399</v>
       </c>
       <c r="M100" s="22" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4897,7 +4999,7 @@
         <v>79</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>81</v>
@@ -4918,7 +5020,7 @@
         <v>0.485</v>
       </c>
       <c r="M101" s="22" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4926,28 +5028,28 @@
         <v>26</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L102" s="4" t="n">
         <v>0.095</v>
       </c>
       <c r="M102" s="22" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4955,19 +5057,19 @@
         <v>71</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>77</v>
@@ -4976,7 +5078,7 @@
         <v>0.827</v>
       </c>
       <c r="M103" s="22" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4984,7 +5086,7 @@
         <v>17</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>19</v>
@@ -4993,7 +5095,7 @@
         <v>20</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>97</v>
@@ -5008,7 +5110,7 @@
         <v>0.095</v>
       </c>
       <c r="M104" s="22" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5016,22 +5118,22 @@
         <v>54</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="L105" s="4" t="n">
         <v>0.304</v>
       </c>
       <c r="M105" s="22" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5039,30 +5141,30 @@
         <v>54</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="L106" s="4" t="n">
         <v>0.352</v>
       </c>
       <c r="M106" s="22" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>94</v>
@@ -5074,39 +5176,39 @@
         <v>46</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L107" s="4" t="n">
         <v>0.247</v>
       </c>
       <c r="M107" s="22" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L108" s="4" t="n">
         <v>0.979</v>
       </c>
       <c r="M108" s="22" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5114,7 +5216,7 @@
         <v>17</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>19</v>
@@ -5123,7 +5225,7 @@
         <v>20</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>97</v>
@@ -5138,7 +5240,7 @@
         <v>0.095</v>
       </c>
       <c r="M109" s="22" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,19 +5248,19 @@
         <v>79</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H110" s="2" t="s">
         <v>46</v>
@@ -5167,7 +5269,7 @@
         <v>3.5</v>
       </c>
       <c r="M110" s="22" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5175,10 +5277,10 @@
         <v>26</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>20</v>
@@ -5190,65 +5292,65 @@
         <v>30</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L111" s="4" t="n">
         <v>0.095</v>
       </c>
       <c r="M111" s="22" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L112" s="4" t="n">
         <v>0.494</v>
       </c>
       <c r="M112" s="22" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L113" s="4" t="n">
         <v>0.57</v>
       </c>
       <c r="M113" s="22" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5256,7 +5358,7 @@
         <v>26</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>102</v>
@@ -5265,7 +5367,7 @@
         <v>20</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>22</v>
@@ -5277,33 +5379,33 @@
         <v>0.095</v>
       </c>
       <c r="M114" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L115" s="4" t="n">
         <v>0.285</v>
       </c>
       <c r="M115" s="5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,22 +5413,22 @@
         <v>54</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="L116" s="4" t="n">
         <v>0.39</v>
       </c>
       <c r="M116" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5334,16 +5436,16 @@
         <v>17</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>97</v>
@@ -5352,65 +5454,65 @@
         <v>23</v>
       </c>
       <c r="I117" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L117" s="4" t="n">
         <v>0.58</v>
       </c>
       <c r="M117" s="5" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L118" s="4" t="n">
         <v>0.247</v>
       </c>
       <c r="M118" s="5" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L119" s="4" t="n">
         <v>0.114</v>
       </c>
       <c r="M119" s="5" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5418,7 +5520,7 @@
         <v>33</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>35</v>
@@ -5427,19 +5529,19 @@
         <v>36</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="L120" s="4" t="n">
         <v>5</v>
       </c>
       <c r="M120" s="5" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5447,28 +5549,28 @@
         <v>79</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="L121" s="4" t="n">
         <v>1.23</v>
       </c>
       <c r="M121" s="5" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5476,7 +5578,7 @@
         <v>26</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>102</v>
@@ -5485,7 +5587,7 @@
         <v>20</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>30</v>
@@ -5497,7 +5599,7 @@
         <v>0.095</v>
       </c>
       <c r="M122" s="5" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5505,7 +5607,7 @@
         <v>26</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>28</v>
@@ -5514,19 +5616,19 @@
         <v>20</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L123" s="4" t="n">
         <v>0.219</v>
       </c>
       <c r="M123" s="5" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5534,7 +5636,7 @@
         <v>26</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>102</v>
@@ -5543,71 +5645,71 @@
         <v>63</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L124" s="4" t="n">
         <v>0.152</v>
       </c>
       <c r="M124" s="5" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="L125" s="4" t="n">
         <v>0.257</v>
       </c>
       <c r="M125" s="5" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="L126" s="4" t="n">
         <v>1.07</v>
       </c>
       <c r="M126" s="5" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5615,16 +5717,16 @@
         <v>17</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>22</v>
@@ -5639,7 +5741,7 @@
         <v>0.095</v>
       </c>
       <c r="M127" s="5" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5647,19 +5749,19 @@
         <v>26</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>23</v>
@@ -5668,7 +5770,7 @@
         <v>1.05</v>
       </c>
       <c r="M128" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5676,22 +5778,22 @@
         <v>54</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="L129" s="4" t="n">
         <v>0.124</v>
       </c>
       <c r="M129" s="5" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5699,19 +5801,19 @@
         <v>26</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>23</v>
@@ -5720,7 +5822,7 @@
         <v>0.095</v>
       </c>
       <c r="M130" s="5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5728,13 +5830,13 @@
         <v>41</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>45</v>
@@ -5743,13 +5845,13 @@
         <v>82</v>
       </c>
       <c r="H131" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="L131" s="4" t="n">
         <v>5.97</v>
       </c>
       <c r="M131" s="5" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5757,81 +5859,304 @@
         <v>26</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H132" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L132" s="4" t="n">
         <v>0.143</v>
       </c>
       <c r="M132" s="5" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="L133" s="4" t="n">
         <v>0.257</v>
       </c>
       <c r="M133" s="5" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L134" s="4" t="n">
         <v>0.095</v>
       </c>
       <c r="M134" s="5" t="s">
-        <v>516</v>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="L135" s="4" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="M135" s="5" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="L136" s="4" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="M136" s="5" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L137" s="4" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="M137" s="5" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I138" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L138" s="4" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="M138" s="5" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="L139" s="4" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="M139" s="5" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="L140" s="4" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="M140" s="5" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L141" s="4" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="M141" s="5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="L142" s="4" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M142" s="5" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B6:M134"/>
+  <autoFilter ref="B6:M143"/>
   <hyperlinks>
     <hyperlink ref="M7" r:id="rId1" display="https://nl.mouser.com/ProductDetail/Vishay-Dale/CRCW04022K20JNED?qs=hD42E%2F8yzjr994JNQ8Enjw%3D%3D"/>
     <hyperlink ref="M8" r:id="rId2" display="https://nl.mouser.com/ProductDetail/KYOCERA-AVX/04026C104KAT2A?qs=Q0wCMCRSJ1vLqipDGm0h%252BA%3D%3D"/>
@@ -5961,6 +6286,14 @@
     <hyperlink ref="M132" r:id="rId126" display="https://nl.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL31B475KAHNNNE?qs=349EhDEZ59oSE8dT4yS8Ow%3D%3D"/>
     <hyperlink ref="M133" r:id="rId127" display="https://nl.mouser.com/ProductDetail/Texas-Instruments/LM339LVPWR?qs=QNEnbhJQKvZwu88lvYobUw%3D%3D"/>
     <hyperlink ref="M134" r:id="rId128" display="https://nl.mouser.com/ProductDetail/Texas-Instruments/LM321LVIDCKR?qs=qSfuJ%252Bfl%2Fd6RcyTOjkRx5Q%3D%3D"/>
+    <hyperlink ref="M135" r:id="rId129" display="https://nl.mouser.com/ProductDetail/CK/PTS636-SL50-SMTR-LFS?qs=vLWxofP3U2zRoRV76Po6zQ%3D%3D"/>
+    <hyperlink ref="M136" r:id="rId130" display="https://nl.mouser.com/ProductDetail/Kingbright/WP7113ID?qs=hyavMCx%252BcmDJhCThgY7pfQ%3D%3D"/>
+    <hyperlink ref="M137" r:id="rId131" display="https://nl.mouser.com/ProductDetail/Murata-Electronics/BLM18KG101TN1D?qs=MY6wChARw2zdno9LTSL6Ng%3D%3D"/>
+    <hyperlink ref="M138" r:id="rId132" display="https://nl.mouser.com/ProductDetail/Bourns/CAY16-681J4LF?qs=fd0Ij%252BN8svzpg8SscutFRQ%3D%3D"/>
+    <hyperlink ref="M139" r:id="rId133" display="https://nl.mouser.com/ProductDetail/Nexperia/PESD5Z5.0F?qs=HNBw3F7vE2wb3Eh3cMl6Jg%3D%3D"/>
+    <hyperlink ref="M140" r:id="rId134" display="https://nl.mouser.com/ProductDetail/Kingbright/WP7113ND?qs=CJFmpBjNieP5MCFQ3vDfmg%3D%3D"/>
+    <hyperlink ref="M141" r:id="rId135" display="https://nl.mouser.com/ProductDetail/Kingbright/WP7113GD?qs=pz0eHrWKk7njL1kTYKysuw%3D%3D"/>
+    <hyperlink ref="M142" r:id="rId136" display="https://nl.mouser.com/ProductDetail/Microchip-Technology/ATTINY9-TS8R?qs=%2Fqzd9s%252BcLd6Ex7DNcGSsRA%3D%3D"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5969,6 +6302,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId129"/>
+  <drawing r:id="rId137"/>
 </worksheet>
 </file>
</xml_diff>